<commit_message>
sửa lại import phạm vi đi tuyến dùng mã tự sinh
</commit_message>
<xml_diff>
--- a/DMS/Templates/Template_AppUser_Store.xlsx
+++ b/DMS/Templates/Template_AppUser_Store.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5D9FA8-52B9-4FE6-810A-989FC3339CFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BD264C-52C5-4093-9655-96513A9E6884}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>STT</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>{{AppUsers.DisplayName}}</t>
-  </si>
-  <si>
-    <t>{{AppUsers.AppUserStoreMappings.CodeDraft}}</t>
   </si>
   <si>
     <t>{{AppUsers.AppUserStoreMappings.Code}}</t>
@@ -439,7 +436,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +449,7 @@
     <col min="6" max="6" width="42.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -486,10 +483,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>